<commit_message>
Auto stash before merge of "dev-robert" and "origin/development"
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/PersonaGegevens.xlsx
+++ b/api/src/DataFixtures/resources/PersonaGegevens.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\brpservice\api\src\DataFixtures\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF8B8E7-1996-41A8-B40C-368E341A1744}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5C55CC-7D1B-42F4-9E7C-8F1D2686205E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4FACEB62-5131-4109-9E05-7E847D4BADD6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4FACEB62-5131-4109-9E05-7E847D4BADD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="98">
   <si>
     <t>Martin Timmers</t>
   </si>
@@ -311,13 +311,64 @@
   </si>
   <si>
     <t>3de of 4de  graad familie</t>
+  </si>
+  <si>
+    <t>koppel4</t>
+  </si>
+  <si>
+    <t>Luuk Noord</t>
+  </si>
+  <si>
+    <t>Leyah Hanzen</t>
+  </si>
+  <si>
+    <t>Luuk</t>
+  </si>
+  <si>
+    <t>Leyah</t>
+  </si>
+  <si>
+    <t>Noord</t>
+  </si>
+  <si>
+    <t>Hanzen</t>
+  </si>
+  <si>
+    <t>Uddel</t>
+  </si>
+  <si>
+    <t>Dorpsstraat</t>
+  </si>
+  <si>
+    <t>Wagenweg</t>
+  </si>
+  <si>
+    <t>Swalmen</t>
+  </si>
+  <si>
+    <t>5953 AG</t>
+  </si>
+  <si>
+    <t>3852 NR</t>
+  </si>
+  <si>
+    <t>lightside@e-mail.com</t>
+  </si>
+  <si>
+    <t>06-12873477</t>
+  </si>
+  <si>
+    <t>darkside@e-mail.com</t>
+  </si>
+  <si>
+    <t>06-12873488</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -355,6 +406,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,10 +540,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -592,8 +652,12 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -926,10 +990,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE223CDD-1CDF-48DE-B60D-3D4711D29029}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="128.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1383,9 +1447,134 @@
         <v>57</v>
       </c>
     </row>
+    <row r="8" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="28"/>
+      <c r="F8" s="31">
+        <v>999999887</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="37">
+        <v>29983</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="33" t="s">
+        <v>89</v>
+      </c>
+      <c r="M8" s="38">
+        <v>4</v>
+      </c>
+      <c r="N8" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="O8" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="P8" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="R8" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="S8" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>87</v>
+      </c>
+      <c r="E9" s="28"/>
+      <c r="F9" s="31">
+        <v>999999888</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="37">
+        <v>30349</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="33" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="38">
+        <v>22</v>
+      </c>
+      <c r="N9" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="O9" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="P9" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q9" s="39" t="s">
+        <v>96</v>
+      </c>
+      <c r="R9" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="T9" s="23" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="Q8" r:id="rId1" xr:uid="{9934B58A-F488-4849-8040-07EAC2836FCE}"/>
+    <hyperlink ref="Q9" r:id="rId2" xr:uid="{027E1B48-05B7-4833-91C4-D7C3EB98F791}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixje en digid testnoodpersonen
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/PersonaGegevens.xlsx
+++ b/api/src/DataFixtures/resources/PersonaGegevens.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rjzon\Documents\Conduction\brpservice\api\src\DataFixtures\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\Conduction\Repos\brpservice\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679A86B2-2090-4DD6-A195-E778BC32FAC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451F934B-E468-40A8-94A1-EB044C5B77BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{4FACEB62-5131-4109-9E05-7E847D4BADD6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4FACEB62-5131-4109-9E05-7E847D4BADD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad2" sheetId="2" r:id="rId1"/>
     <sheet name="Blad1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" refMode="R1C1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="140">
   <si>
     <t>Koppel</t>
   </si>
@@ -454,13 +454,49 @@
   </si>
   <si>
     <t>4-4-1985</t>
+  </si>
+  <si>
+    <t>Angeline</t>
+  </si>
+  <si>
+    <t>Vogel</t>
+  </si>
+  <si>
+    <t>Teststraat</t>
+  </si>
+  <si>
+    <t>1000AA</t>
+  </si>
+  <si>
+    <t>Tobias</t>
+  </si>
+  <si>
+    <t>Kat</t>
+  </si>
+  <si>
+    <t>Renate</t>
+  </si>
+  <si>
+    <t>Hond</t>
+  </si>
+  <si>
+    <t>Piet</t>
+  </si>
+  <si>
+    <t>Koe</t>
+  </si>
+  <si>
+    <t>Petra</t>
+  </si>
+  <si>
+    <t>Giraf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +542,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,7 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -798,6 +841,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1136,7 +1192,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="128.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1830,20 +1886,160 @@
         <v>32</v>
       </c>
     </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12"/>
+      <c r="F12" s="57">
+        <v>900220806</v>
+      </c>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M12" s="59">
+        <v>1</v>
+      </c>
+      <c r="N12" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="O12" s="58" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13" s="55" t="s">
+        <v>132</v>
+      </c>
+      <c r="D13" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13" s="57">
+        <v>900220818</v>
+      </c>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M13" s="59">
+        <v>1</v>
+      </c>
+      <c r="N13" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="O13" s="58" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14"/>
+      <c r="C14" s="55" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14" s="57">
+        <v>900220831</v>
+      </c>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M14" s="59">
+        <v>1</v>
+      </c>
+      <c r="N14" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="O14" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15"/>
+      <c r="C15" s="55" t="s">
+        <v>136</v>
+      </c>
+      <c r="D15" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15" s="57">
+        <v>900220843</v>
+      </c>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M15" s="59">
+        <v>1</v>
+      </c>
+      <c r="N15" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="O15" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16"/>
+      <c r="C16" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="D16" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16" s="57">
+        <v>900220855</v>
+      </c>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="M16" s="59">
+        <v>1</v>
+      </c>
+      <c r="N16" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="O16" s="58" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17"/>

</xml_diff>

<commit_message>
Temporarily only load test personas for digid
</commit_message>
<xml_diff>
--- a/api/src/DataFixtures/resources/PersonaGegevens.xlsx
+++ b/api/src/DataFixtures/resources/PersonaGegevens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\Conduction\Repos\brpservice\api\src\DataFixtures\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{451F934B-E468-40A8-94A1-EB044C5B77BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC07F0AE-A1C2-4AAF-9D35-838652D5207D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{4FACEB62-5131-4109-9E05-7E847D4BADD6}"/>
   </bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="116">
   <si>
     <t>Koppel</t>
   </si>
@@ -318,63 +318,9 @@
     <t>koppel4</t>
   </si>
   <si>
-    <t>Luuk Noord</t>
-  </si>
-  <si>
-    <t>Luuk</t>
-  </si>
-  <si>
-    <t>Noord</t>
-  </si>
-  <si>
-    <t>Swalmen</t>
-  </si>
-  <si>
-    <t>Dorpsstraat</t>
-  </si>
-  <si>
-    <t>5953 AG</t>
-  </si>
-  <si>
-    <t>lightside@e-mail.com</t>
-  </si>
-  <si>
-    <t>06-12873477</t>
-  </si>
-  <si>
-    <t>Leyah Hanzen</t>
-  </si>
-  <si>
-    <t>Leyah</t>
-  </si>
-  <si>
-    <t>Hanzen</t>
-  </si>
-  <si>
-    <t>Uddel</t>
-  </si>
-  <si>
-    <t>Wagenweg</t>
-  </si>
-  <si>
-    <t>3852 NR</t>
-  </si>
-  <si>
-    <t>darkside@e-mail.com</t>
-  </si>
-  <si>
-    <t>06-12873488</t>
-  </si>
-  <si>
-    <t>koppel5</t>
-  </si>
-  <si>
     <t>Michelle Dautzenberg</t>
   </si>
   <si>
-    <t>Michelle</t>
-  </si>
-  <si>
     <t>Dautzenberg</t>
   </si>
   <si>
@@ -387,9 +333,6 @@
     <t>1357 CP</t>
   </si>
   <si>
-    <t>Michelle@email.com</t>
-  </si>
-  <si>
     <t>06-44478969</t>
   </si>
   <si>
@@ -411,9 +354,6 @@
     <t>1012 VM</t>
   </si>
   <si>
-    <t>Rick@email.com</t>
-  </si>
-  <si>
     <t>06-88474321</t>
   </si>
   <si>
@@ -426,36 +366,6 @@
     <t>rick@email.com</t>
   </si>
   <si>
-    <t>4-3-1951</t>
-  </si>
-  <si>
-    <t>1-2-1958</t>
-  </si>
-  <si>
-    <t>16-4-1982</t>
-  </si>
-  <si>
-    <t>24-11-1977</t>
-  </si>
-  <si>
-    <t>17-7-1986</t>
-  </si>
-  <si>
-    <t>26-9-1990</t>
-  </si>
-  <si>
-    <t>1-2-1982</t>
-  </si>
-  <si>
-    <t>2-2-1983</t>
-  </si>
-  <si>
-    <t>3-3-1984</t>
-  </si>
-  <si>
-    <t>4-4-1985</t>
-  </si>
-  <si>
     <t>Angeline</t>
   </si>
   <si>
@@ -490,13 +400,31 @@
   </si>
   <si>
     <t>Giraf</t>
+  </si>
+  <si>
+    <t>900220806</t>
+  </si>
+  <si>
+    <t>900220818</t>
+  </si>
+  <si>
+    <t>900220831</t>
+  </si>
+  <si>
+    <t>900220843</t>
+  </si>
+  <si>
+    <t>900220855</t>
+  </si>
+  <si>
+    <t>1-1-1960</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +477,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -703,7 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -783,16 +717,10 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -847,13 +775,14 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1192,7 +1121,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="128.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1150,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="24" t="s">
@@ -1230,13 +1159,13 @@
       <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="29" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="24" t="s">
@@ -1254,16 +1183,16 @@
       <c r="K1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="29" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="30" t="s">
+      <c r="O1" s="29" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="24" t="s">
@@ -1282,764 +1211,325 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="28"/>
-      <c r="F2" s="31">
-        <v>999999837</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="54" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="37">
-        <v>5</v>
-      </c>
-      <c r="N2" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="23" t="s">
-        <v>32</v>
-      </c>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="33"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="53" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="G2"/>
+      <c r="H2" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="56">
+        <v>1</v>
+      </c>
+      <c r="N2" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="31">
-        <v>999999850</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="54" t="s">
-        <v>119</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K3" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L3" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" s="37">
-        <v>10</v>
-      </c>
-      <c r="N3" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="O3" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="A3" s="33"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="53" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3"/>
+      <c r="F3" s="57" t="s">
+        <v>111</v>
+      </c>
+      <c r="G3"/>
+      <c r="H3" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="56">
+        <v>1</v>
+      </c>
+      <c r="N3" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="31">
-        <v>999999230</v>
-      </c>
-      <c r="G4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H4" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="I4" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="M4" s="37">
+      <c r="A4" s="33"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="53" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="54" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4"/>
+      <c r="F4" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4"/>
+      <c r="H4" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M4" s="56">
         <v>1</v>
       </c>
-      <c r="N4" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="O4" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="R4" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="S4" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T4" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>57</v>
-      </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="32">
-        <v>999997865</v>
-      </c>
-      <c r="G5" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H5" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="I5" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="L5" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="37">
+      <c r="N4" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="23"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="53" t="s">
+        <v>106</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5"/>
+      <c r="F5" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M5" s="56">
         <v>1</v>
       </c>
-      <c r="N5" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="O5" s="33" t="s">
-        <v>52</v>
-      </c>
-      <c r="P5" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="R5" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="S5" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="23" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="E6" s="28"/>
-      <c r="F6" s="31">
-        <v>999999928</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H6" s="54" t="s">
-        <v>122</v>
-      </c>
-      <c r="I6" s="23" t="s">
+      <c r="N5" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="J6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L6" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="M6" s="37">
-        <v>60</v>
-      </c>
-      <c r="N6" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="O6" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="P6" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="R6" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="S6" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T6" s="23" t="s">
-        <v>73</v>
-      </c>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="53" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6"/>
+      <c r="F6" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="M6" s="56">
+        <v>1</v>
+      </c>
+      <c r="N6" s="55" t="s">
+        <v>101</v>
+      </c>
+      <c r="O6" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="23"/>
     </row>
     <row r="7" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="31" t="s">
-        <v>76</v>
-      </c>
+      <c r="A7" s="34"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="30"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="31">
-        <v>999999886</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="54" t="s">
-        <v>123</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>78</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="M7" s="37">
-        <v>60</v>
-      </c>
-      <c r="N7" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="O7" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="P7" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="R7" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="S7" s="23" t="s">
-        <v>73</v>
-      </c>
-      <c r="T7" s="23" t="s">
-        <v>73</v>
-      </c>
+      <c r="F7" s="30"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="35"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
     </row>
     <row r="8" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="31" t="s">
-        <v>84</v>
-      </c>
+      <c r="A8" s="33"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="30"/>
       <c r="E8" s="28"/>
-      <c r="F8" s="31">
-        <v>999999887</v>
-      </c>
-      <c r="G8" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="54" t="s">
-        <v>124</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L8" s="33" t="s">
-        <v>86</v>
-      </c>
-      <c r="M8" s="37">
-        <v>4</v>
-      </c>
-      <c r="N8" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="O8" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="P8" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q8" s="38" t="s">
-        <v>88</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="S8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T8" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="F8" s="30"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="23"/>
+      <c r="Q8" s="36"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
     </row>
     <row r="9" spans="1:20" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="26" t="s">
-        <v>91</v>
-      </c>
-      <c r="D9" s="31" t="s">
-        <v>92</v>
-      </c>
-      <c r="E9" s="46"/>
-      <c r="F9" s="31">
-        <v>999999888</v>
-      </c>
-      <c r="G9" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="H9" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="M9" s="37">
-        <v>22</v>
-      </c>
-      <c r="N9" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="O9" s="43" t="s">
-        <v>93</v>
-      </c>
-      <c r="P9" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q9" s="38" t="s">
-        <v>96</v>
-      </c>
-      <c r="R9" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="S9" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="T9" s="23" t="s">
-        <v>32</v>
-      </c>
+      <c r="A9" s="33"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="41"/>
+      <c r="P9" s="23"/>
+      <c r="Q9" s="36"/>
+      <c r="R9" s="23"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="23"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B10" s="39" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="44" t="s">
-        <v>101</v>
-      </c>
-      <c r="E10" s="47"/>
-      <c r="F10" s="45">
-        <v>999999889</v>
-      </c>
-      <c r="G10" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>102</v>
-      </c>
-      <c r="J10" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="K10" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="L10" s="44" t="s">
-        <v>103</v>
-      </c>
-      <c r="M10" s="41">
-        <v>149</v>
-      </c>
-      <c r="N10" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="O10" s="44" t="s">
-        <v>102</v>
-      </c>
-      <c r="P10" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q10" s="40" t="s">
-        <v>105</v>
-      </c>
-      <c r="R10" s="39" t="s">
-        <v>106</v>
-      </c>
-      <c r="S10" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="T10" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="A10" s="37"/>
+      <c r="B10" s="37"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="37"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="42"/>
+      <c r="O10" s="42"/>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="38"/>
+      <c r="R10" s="37"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="37"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="39" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="47"/>
-      <c r="F11" s="45">
-        <v>999999890</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="H11" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>110</v>
-      </c>
-      <c r="J11" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="K11" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>111</v>
-      </c>
-      <c r="M11" s="41">
-        <v>12</v>
-      </c>
-      <c r="N11" s="44" t="s">
-        <v>112</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>110</v>
-      </c>
-      <c r="P11" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q11" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="R11" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="S11" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="T11" s="39" t="s">
-        <v>32</v>
-      </c>
+      <c r="A11" s="37"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="37"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="39"/>
+      <c r="N11" s="42"/>
+      <c r="O11" s="42"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="37"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
-      <c r="C12" s="55" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="E12"/>
-      <c r="F12" s="57">
-        <v>900220806</v>
-      </c>
-      <c r="G12"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="M12" s="59">
-        <v>1</v>
-      </c>
-      <c r="N12" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O12" s="58" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
-      <c r="C13" s="55" t="s">
-        <v>132</v>
-      </c>
-      <c r="D13" s="56" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13"/>
-      <c r="F13" s="57">
-        <v>900220818</v>
-      </c>
-      <c r="G13"/>
-      <c r="H13"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="M13" s="59">
-        <v>1</v>
-      </c>
-      <c r="N13" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O13" s="58" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
-      <c r="C14" s="55" t="s">
-        <v>134</v>
-      </c>
-      <c r="D14" s="56" t="s">
-        <v>135</v>
-      </c>
-      <c r="E14"/>
-      <c r="F14" s="57">
-        <v>900220831</v>
-      </c>
-      <c r="G14"/>
-      <c r="H14"/>
-      <c r="I14"/>
-      <c r="J14"/>
-      <c r="K14"/>
-      <c r="L14" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="M14" s="59">
-        <v>1</v>
-      </c>
-      <c r="N14" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O14" s="58" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
-      <c r="C15" s="55" t="s">
-        <v>136</v>
-      </c>
-      <c r="D15" s="56" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15"/>
-      <c r="F15" s="57">
-        <v>900220843</v>
-      </c>
-      <c r="G15"/>
-      <c r="H15"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="M15" s="59">
-        <v>1</v>
-      </c>
-      <c r="N15" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O15" s="58" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
-      <c r="C16" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="D16" s="56" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16"/>
-      <c r="F16" s="57">
-        <v>900220855</v>
-      </c>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="M16" s="59">
-        <v>1</v>
-      </c>
-      <c r="N16" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="O16" s="58" t="s">
-        <v>67</v>
-      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17"/>
@@ -2097,15 +1587,10 @@
       <c r="C27"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="Q8" r:id="rId1" xr:uid="{9934B58A-F488-4849-8040-07EAC2836FCE}"/>
-    <hyperlink ref="Q9" r:id="rId2" xr:uid="{027E1B48-05B7-4833-91C4-D7C3EB98F791}"/>
-    <hyperlink ref="Q10" r:id="rId3" xr:uid="{19CDBB78-C69F-48B4-A532-143E00C6CECA}"/>
-    <hyperlink ref="Q11" r:id="rId4" xr:uid="{2CCEA01A-F180-4756-95FF-3791D00A6B50}"/>
-  </hyperlinks>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
-  <legacyDrawing r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2145,10 +1630,10 @@
       <c r="G1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="46" t="s">
         <v>81</v>
       </c>
     </row>
@@ -2174,11 +1659,11 @@
       <c r="G2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H2" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="I2" s="48" t="s">
-        <v>107</v>
+      <c r="H2" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="I2" s="46" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2203,11 +1688,11 @@
       <c r="G3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="48" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" s="48" t="s">
-        <v>108</v>
+      <c r="H3" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -2232,11 +1717,11 @@
       <c r="G4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="48" t="s">
-        <v>101</v>
-      </c>
-      <c r="I4" s="48" t="s">
-        <v>109</v>
+      <c r="H4" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
@@ -2253,8 +1738,8 @@
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
@@ -2278,10 +1763,10 @@
       <c r="G6" s="11">
         <v>999999886</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="47">
         <v>999999889</v>
       </c>
-      <c r="I6" s="49">
+      <c r="I6" s="47">
         <v>999999890</v>
       </c>
     </row>
@@ -2307,10 +1792,10 @@
       <c r="G7" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="48" t="s">
+      <c r="H7" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="46" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2336,10 +1821,10 @@
       <c r="G8" s="17">
         <v>33142</v>
       </c>
-      <c r="H8" s="50">
+      <c r="H8" s="48">
         <v>30744</v>
       </c>
-      <c r="I8" s="50">
+      <c r="I8" s="48">
         <v>31141</v>
       </c>
     </row>
@@ -2365,11 +1850,11 @@
       <c r="G9" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="H9" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="I9" s="48" t="s">
-        <v>110</v>
+      <c r="H9" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" s="46" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2394,10 +1879,10 @@
       <c r="G10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H10" s="48" t="s">
+      <c r="H10" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="46" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2423,10 +1908,10 @@
       <c r="G11" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H11" s="48" t="s">
+      <c r="H11" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="46" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2452,11 +1937,11 @@
       <c r="G12" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H12" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="I12" s="48" t="s">
-        <v>111</v>
+      <c r="H12" s="46" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="46" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2481,10 +1966,10 @@
       <c r="G13" s="19">
         <v>60</v>
       </c>
-      <c r="H13" s="51">
+      <c r="H13" s="49">
         <v>149</v>
       </c>
-      <c r="I13" s="51">
+      <c r="I13" s="49">
         <v>12</v>
       </c>
     </row>
@@ -2510,11 +1995,11 @@
       <c r="G14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="52" t="s">
-        <v>104</v>
-      </c>
-      <c r="I14" s="52" t="s">
-        <v>112</v>
+      <c r="H14" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" s="50" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2539,11 +2024,11 @@
       <c r="G15" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="H15" s="48" t="s">
-        <v>102</v>
-      </c>
-      <c r="I15" s="48" t="s">
-        <v>110</v>
+      <c r="H15" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="46" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -2568,10 +2053,10 @@
       <c r="G16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="46" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2597,11 +2082,11 @@
       <c r="G17" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="H17" s="53" t="s">
-        <v>116</v>
-      </c>
-      <c r="I17" s="53" t="s">
-        <v>117</v>
+      <c r="H17" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="I17" s="51" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2626,11 +2111,11 @@
       <c r="G18" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="H18" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="I18" s="52" t="s">
-        <v>114</v>
+      <c r="H18" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="50" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -2655,10 +2140,10 @@
       <c r="G19" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I19" s="48" t="s">
+      <c r="I19" s="46" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2684,10 +2169,10 @@
       <c r="G20" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="H20" s="48" t="s">
+      <c r="H20" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="46" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>